<commit_message>
not sure if anything was changed here, but resaved.
</commit_message>
<xml_diff>
--- a/Template_Files/02_HazardAnalysisAndRiskAssessment_Template.xlsx
+++ b/Template_Files/02_HazardAnalysisAndRiskAssessment_Template.xlsx
@@ -1509,8 +1509,8 @@
   </sheetPr>
   <dimension ref="A1:AB16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W22" activeCellId="0" sqref="W22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>